<commit_message>
Se agrega clase php para cerrar la sesión, además se prepara otro para modificar usuario
</commit_message>
<xml_diff>
--- a/documentacion/Lista Requerimientos proyecto.xlsx
+++ b/documentacion/Lista Requerimientos proyecto.xlsx
@@ -1,15 +1,15 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
-  <workbookPr defaultThemeVersion="153222"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="18827"/>
+  <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\xampp\htdocs\Proyecto_ ISW-611\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\xampp\htdocs\Proyecto_ ISW-611\documentacion\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="20490" windowHeight="7755"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="20490" windowHeight="7755" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Hoja1" sheetId="1" r:id="rId1"/>
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="222" uniqueCount="135">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="223" uniqueCount="136">
   <si>
     <t>Descripción</t>
   </si>
@@ -296,9 +296,6 @@
     <t xml:space="preserve"> RS-001</t>
   </si>
   <si>
-    <t>Esta es la primera pantalla que se mostrara</t>
-  </si>
-  <si>
     <t>Pequeño formulario que solicita correo, fecha nacimiento y respuesta a pregunta de recuperación, si los 3 datos son contestados correctamente envia la contraseña anterior al correo electronico, y solicitara hacer cambio de contraseña</t>
   </si>
   <si>
@@ -429,12 +426,18 @@
   </si>
   <si>
     <t xml:space="preserve"> RS-001, RS-009</t>
+  </si>
+  <si>
+    <t>Pendiente el flujo de ocultarse el formulario</t>
+  </si>
+  <si>
+    <t>Pendiente  botones de olvido y regristrar el usuario</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <fonts count="1" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -444,7 +447,7 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="3">
+  <fills count="4">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -454,6 +457,12 @@
     <fill>
       <patternFill patternType="solid">
         <fgColor theme="4" tint="0.59999389629810485"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="-0.249977111117893"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -470,7 +479,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="6">
+  <cellXfs count="7">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment wrapText="1"/>
@@ -486,6 +495,9 @@
     </xf>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment vertical="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -527,23 +539,23 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="1" name="Tabla1" displayName="Tabla1" ref="A1:K26" totalsRowShown="0">
-  <autoFilter ref="A1:K26"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{00000000-000C-0000-FFFF-FFFF00000000}" name="Tabla1" displayName="Tabla1" ref="A1:K26" totalsRowShown="0">
+  <autoFilter ref="A1:K26" xr:uid="{00000000-0009-0000-0100-000001000000}"/>
   <sortState ref="A2:K19">
     <sortCondition ref="A1:A19"/>
   </sortState>
   <tableColumns count="11">
-    <tableColumn id="1" name="# R" dataDxfId="6"/>
-    <tableColumn id="2" name="Nombre Requerimiento" dataDxfId="5"/>
-    <tableColumn id="3" name="Version" dataDxfId="4"/>
-    <tableColumn id="4" name="Autor" dataDxfId="3"/>
-    <tableColumn id="5" name="Requisitos Asociados" dataDxfId="2"/>
-    <tableColumn id="6" name="Descripción" dataDxfId="1"/>
-    <tableColumn id="7" name="Precondición" dataDxfId="0"/>
-    <tableColumn id="8" name="Secuencia Normal"/>
-    <tableColumn id="9" name="Post Condicion"/>
-    <tableColumn id="10" name="Importancia"/>
-    <tableColumn id="11" name="Comentarios"/>
+    <tableColumn id="1" xr3:uid="{00000000-0010-0000-0000-000001000000}" name="# R" dataDxfId="6"/>
+    <tableColumn id="2" xr3:uid="{00000000-0010-0000-0000-000002000000}" name="Nombre Requerimiento" dataDxfId="5"/>
+    <tableColumn id="3" xr3:uid="{00000000-0010-0000-0000-000003000000}" name="Version" dataDxfId="4"/>
+    <tableColumn id="4" xr3:uid="{00000000-0010-0000-0000-000004000000}" name="Autor" dataDxfId="3"/>
+    <tableColumn id="5" xr3:uid="{00000000-0010-0000-0000-000005000000}" name="Requisitos Asociados" dataDxfId="2"/>
+    <tableColumn id="6" xr3:uid="{00000000-0010-0000-0000-000006000000}" name="Descripción" dataDxfId="1"/>
+    <tableColumn id="7" xr3:uid="{00000000-0010-0000-0000-000007000000}" name="Precondición" dataDxfId="0"/>
+    <tableColumn id="8" xr3:uid="{00000000-0010-0000-0000-000008000000}" name="Secuencia Normal"/>
+    <tableColumn id="9" xr3:uid="{00000000-0010-0000-0000-000009000000}" name="Post Condicion"/>
+    <tableColumn id="10" xr3:uid="{00000000-0010-0000-0000-00000A000000}" name="Importancia"/>
+    <tableColumn id="11" xr3:uid="{00000000-0010-0000-0000-00000B000000}" name="Comentarios"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleLight9" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
@@ -811,11 +823,11 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:K26"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A12" workbookViewId="0">
-      <selection activeCell="H15" sqref="H15"/>
+    <sheetView tabSelected="1" topLeftCell="A3" workbookViewId="0">
+      <selection activeCell="K5" sqref="K5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -826,11 +838,11 @@
     <col min="4" max="4" width="14" bestFit="1" customWidth="1"/>
     <col min="5" max="5" width="5.85546875" customWidth="1"/>
     <col min="6" max="6" width="24.42578125" customWidth="1"/>
-    <col min="7" max="7" width="14.85546875" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="14.85546875" hidden="1" customWidth="1"/>
     <col min="8" max="8" width="46.42578125" customWidth="1"/>
-    <col min="9" max="9" width="15.140625" customWidth="1"/>
-    <col min="10" max="10" width="13.7109375" customWidth="1"/>
-    <col min="11" max="11" width="14.42578125" customWidth="1"/>
+    <col min="9" max="9" width="15.140625" hidden="1" customWidth="1"/>
+    <col min="10" max="10" width="13.7109375" hidden="1" customWidth="1"/>
+    <col min="11" max="11" width="47.140625" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:11" ht="27.75" customHeight="1" x14ac:dyDescent="0.25">
@@ -869,7 +881,7 @@
       </c>
     </row>
     <row r="2" spans="1:11" ht="125.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A2" s="4" t="s">
+      <c r="A2" s="6" t="s">
         <v>49</v>
       </c>
       <c r="B2" s="3" t="s">
@@ -889,14 +901,17 @@
       </c>
       <c r="G2" s="4"/>
       <c r="H2" s="1" t="s">
-        <v>102</v>
+        <v>101</v>
       </c>
       <c r="J2" s="1" t="s">
         <v>15</v>
       </c>
+      <c r="K2" t="s">
+        <v>134</v>
+      </c>
     </row>
     <row r="3" spans="1:11" ht="93.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A3" s="4" t="s">
+      <c r="A3" s="6" t="s">
         <v>50</v>
       </c>
       <c r="B3" s="4" t="s">
@@ -924,7 +939,7 @@
         <v>15</v>
       </c>
       <c r="K3" s="3" t="s">
-        <v>90</v>
+        <v>135</v>
       </c>
     </row>
     <row r="4" spans="1:11" ht="73.5" customHeight="1" x14ac:dyDescent="0.25">
@@ -950,7 +965,7 @@
         <v>50</v>
       </c>
       <c r="H4" s="1" t="s">
-        <v>91</v>
+        <v>90</v>
       </c>
       <c r="J4" t="s">
         <v>21</v>
@@ -970,7 +985,7 @@
         <v>12</v>
       </c>
       <c r="E5" s="4" t="s">
-        <v>98</v>
+        <v>97</v>
       </c>
       <c r="F5" s="3" t="s">
         <v>22</v>
@@ -991,7 +1006,7 @@
         <v>53</v>
       </c>
       <c r="B6" s="3" t="s">
-        <v>92</v>
+        <v>91</v>
       </c>
       <c r="C6" s="4" t="s">
         <v>11</v>
@@ -1001,13 +1016,13 @@
       </c>
       <c r="E6" s="4"/>
       <c r="F6" s="3" t="s">
+        <v>92</v>
+      </c>
+      <c r="G6" s="4" t="s">
         <v>93</v>
       </c>
-      <c r="G6" s="4" t="s">
+      <c r="H6" s="3" t="s">
         <v>94</v>
-      </c>
-      <c r="H6" s="3" t="s">
-        <v>95</v>
       </c>
       <c r="I6" s="4" t="s">
         <v>54</v>
@@ -1036,7 +1051,7 @@
         <v>24</v>
       </c>
       <c r="G7" s="4" t="s">
-        <v>99</v>
+        <v>98</v>
       </c>
       <c r="H7" s="3" t="s">
         <v>26</v>
@@ -1091,7 +1106,7 @@
         <v>12</v>
       </c>
       <c r="E9" s="4" t="s">
-        <v>134</v>
+        <v>133</v>
       </c>
       <c r="F9" s="3" t="s">
         <v>31</v>
@@ -1126,7 +1141,7 @@
         <v>33</v>
       </c>
       <c r="G10" s="3" t="s">
-        <v>96</v>
+        <v>95</v>
       </c>
       <c r="H10" s="1" t="s">
         <v>34</v>
@@ -1155,7 +1170,7 @@
         <v>36</v>
       </c>
       <c r="G11" s="4" t="s">
-        <v>97</v>
+        <v>96</v>
       </c>
       <c r="H11" s="1" t="s">
         <v>37</v>
@@ -1184,7 +1199,7 @@
         <v>40</v>
       </c>
       <c r="G12" s="4" t="s">
-        <v>97</v>
+        <v>96</v>
       </c>
       <c r="H12" s="1" t="s">
         <v>43</v>
@@ -1216,7 +1231,7 @@
         <v>42</v>
       </c>
       <c r="G13" s="4" t="s">
-        <v>97</v>
+        <v>96</v>
       </c>
       <c r="H13" s="1" t="s">
         <v>44</v>
@@ -1242,7 +1257,7 @@
         <v>12</v>
       </c>
       <c r="E14" s="4" t="s">
-        <v>133</v>
+        <v>132</v>
       </c>
       <c r="F14" s="3" t="s">
         <v>68</v>
@@ -1340,7 +1355,7 @@
         <v>81</v>
       </c>
       <c r="B18" s="4" t="s">
-        <v>100</v>
+        <v>99</v>
       </c>
       <c r="C18" s="4" t="s">
         <v>11</v>
@@ -1362,7 +1377,7 @@
     </row>
     <row r="19" spans="1:10" ht="45" x14ac:dyDescent="0.25">
       <c r="A19" s="4" t="s">
-        <v>132</v>
+        <v>131</v>
       </c>
       <c r="B19" s="4" t="s">
         <v>85</v>
@@ -1392,7 +1407,7 @@
         <v>84</v>
       </c>
       <c r="B20" s="4" t="s">
-        <v>125</v>
+        <v>124</v>
       </c>
       <c r="C20" s="4" t="s">
         <v>11</v>
@@ -1404,13 +1419,13 @@
         <v>72</v>
       </c>
       <c r="F20" s="5" t="s">
-        <v>116</v>
+        <v>115</v>
       </c>
       <c r="G20" s="4" t="s">
-        <v>112</v>
+        <v>111</v>
       </c>
       <c r="H20" s="1" t="s">
-        <v>111</v>
+        <v>110</v>
       </c>
       <c r="J20" t="s">
         <v>45</v>
@@ -1418,10 +1433,10 @@
     </row>
     <row r="21" spans="1:10" ht="60" x14ac:dyDescent="0.25">
       <c r="A21" s="4" t="s">
-        <v>101</v>
+        <v>100</v>
       </c>
       <c r="B21" s="4" t="s">
-        <v>124</v>
+        <v>123</v>
       </c>
       <c r="C21" s="4" t="s">
         <v>11</v>
@@ -1431,13 +1446,13 @@
       </c>
       <c r="E21" s="4"/>
       <c r="F21" s="5" t="s">
-        <v>117</v>
+        <v>116</v>
       </c>
       <c r="G21" s="4" t="s">
-        <v>120</v>
+        <v>119</v>
       </c>
       <c r="H21" s="1" t="s">
-        <v>105</v>
+        <v>104</v>
       </c>
       <c r="J21" t="s">
         <v>45</v>
@@ -1445,10 +1460,10 @@
     </row>
     <row r="22" spans="1:10" ht="45" x14ac:dyDescent="0.25">
       <c r="A22" s="4" t="s">
-        <v>103</v>
+        <v>102</v>
       </c>
       <c r="B22" s="4" t="s">
-        <v>123</v>
+        <v>122</v>
       </c>
       <c r="C22" s="4" t="s">
         <v>11</v>
@@ -1458,13 +1473,13 @@
       </c>
       <c r="E22" s="4"/>
       <c r="F22" s="5" t="s">
-        <v>118</v>
+        <v>117</v>
       </c>
       <c r="G22" s="4" t="s">
-        <v>121</v>
+        <v>120</v>
       </c>
       <c r="H22" t="s">
-        <v>104</v>
+        <v>103</v>
       </c>
       <c r="I22" s="4"/>
       <c r="J22" t="s">
@@ -1473,10 +1488,10 @@
     </row>
     <row r="23" spans="1:10" ht="45" x14ac:dyDescent="0.25">
       <c r="A23" s="4" t="s">
+        <v>105</v>
+      </c>
+      <c r="B23" s="4" t="s">
         <v>106</v>
-      </c>
-      <c r="B23" s="4" t="s">
-        <v>107</v>
       </c>
       <c r="C23" s="4" t="s">
         <v>11</v>
@@ -1486,11 +1501,11 @@
       </c>
       <c r="E23" s="4"/>
       <c r="F23" s="5" t="s">
-        <v>109</v>
+        <v>108</v>
       </c>
       <c r="G23" s="4"/>
       <c r="H23" t="s">
-        <v>108</v>
+        <v>107</v>
       </c>
       <c r="J23" t="s">
         <v>21</v>
@@ -1498,10 +1513,10 @@
     </row>
     <row r="24" spans="1:10" ht="48.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A24" s="4" t="s">
-        <v>128</v>
+        <v>127</v>
       </c>
       <c r="B24" s="4" t="s">
-        <v>122</v>
+        <v>121</v>
       </c>
       <c r="C24" s="4" t="s">
         <v>11</v>
@@ -1511,13 +1526,13 @@
       </c>
       <c r="E24" s="4"/>
       <c r="F24" s="5" t="s">
-        <v>119</v>
+        <v>118</v>
       </c>
       <c r="G24" s="4" t="s">
         <v>84</v>
       </c>
       <c r="H24" s="1" t="s">
-        <v>110</v>
+        <v>109</v>
       </c>
       <c r="I24" s="4"/>
       <c r="J24" t="s">
@@ -1526,10 +1541,10 @@
     </row>
     <row r="25" spans="1:10" ht="60" x14ac:dyDescent="0.25">
       <c r="A25" s="4" t="s">
-        <v>127</v>
+        <v>126</v>
       </c>
       <c r="B25" s="4" t="s">
-        <v>113</v>
+        <v>112</v>
       </c>
       <c r="C25" s="4" t="s">
         <v>11</v>
@@ -1539,11 +1554,11 @@
       </c>
       <c r="E25" s="4"/>
       <c r="F25" s="5" t="s">
-        <v>114</v>
+        <v>113</v>
       </c>
       <c r="G25" s="4"/>
       <c r="H25" t="s">
-        <v>115</v>
+        <v>114</v>
       </c>
       <c r="J25" t="s">
         <v>21</v>
@@ -1551,10 +1566,10 @@
     </row>
     <row r="26" spans="1:10" ht="41.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A26" s="4" t="s">
-        <v>126</v>
+        <v>125</v>
       </c>
       <c r="B26" s="4" t="s">
-        <v>130</v>
+        <v>129</v>
       </c>
       <c r="C26" s="4" t="s">
         <v>11</v>
@@ -1564,11 +1579,11 @@
       </c>
       <c r="E26" s="4"/>
       <c r="F26" s="3" t="s">
-        <v>129</v>
+        <v>128</v>
       </c>
       <c r="G26" s="4"/>
       <c r="H26" s="1" t="s">
-        <v>131</v>
+        <v>130</v>
       </c>
       <c r="J26" t="s">
         <v>45</v>

</xml_diff>

<commit_message>
Se trabaja en el formulario de nuevas tareas
</commit_message>
<xml_diff>
--- a/documentacion/Lista Requerimientos proyecto.xlsx
+++ b/documentacion/Lista Requerimientos proyecto.xlsx
@@ -1,13 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="18827"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="19029"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\xampp\htdocs\Proyecto_ ISW-611\documentacion\"/>
     </mc:Choice>
   </mc:AlternateContent>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1DE16A87-AA56-42A9-8283-B18B5535FFAD}" xr6:coauthVersionLast="28" xr6:coauthVersionMax="28" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="20490" windowHeight="7755" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -24,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="223" uniqueCount="136">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="232" uniqueCount="136">
   <si>
     <t>Descripción</t>
   </si>
@@ -428,10 +429,10 @@
     <t xml:space="preserve"> RS-001, RS-009</t>
   </si>
   <si>
-    <t>Pendiente el flujo de ocultarse el formulario</t>
-  </si>
-  <si>
-    <t>Pendiente  botones de olvido y regristrar el usuario</t>
+    <t>Listo</t>
+  </si>
+  <si>
+    <t>Listo, falta olvido contraseña</t>
   </si>
 </sst>
 </file>
@@ -447,7 +448,7 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="4">
+  <fills count="3">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -457,12 +458,6 @@
     <fill>
       <patternFill patternType="solid">
         <fgColor theme="4" tint="0.59999389629810485"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9" tint="-0.249977111117893"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -479,7 +474,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="7">
+  <cellXfs count="6">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment wrapText="1"/>
@@ -495,9 +490,6 @@
     </xf>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
-      <alignment vertical="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -826,8 +818,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:K26"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A3" workbookViewId="0">
-      <selection activeCell="K5" sqref="K5"/>
+    <sheetView tabSelected="1" topLeftCell="A4" workbookViewId="0">
+      <selection activeCell="K8" sqref="K8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -881,7 +873,7 @@
       </c>
     </row>
     <row r="2" spans="1:11" ht="125.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A2" s="6" t="s">
+      <c r="A2" s="4" t="s">
         <v>49</v>
       </c>
       <c r="B2" s="3" t="s">
@@ -911,7 +903,7 @@
       </c>
     </row>
     <row r="3" spans="1:11" ht="93.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A3" s="6" t="s">
+      <c r="A3" s="4" t="s">
         <v>50</v>
       </c>
       <c r="B3" s="4" t="s">
@@ -1030,6 +1022,9 @@
       <c r="J6" t="s">
         <v>15</v>
       </c>
+      <c r="K6" t="s">
+        <v>134</v>
+      </c>
     </row>
     <row r="7" spans="1:11" ht="73.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A7" s="4" t="s">
@@ -1059,6 +1054,9 @@
       <c r="J7" t="s">
         <v>21</v>
       </c>
+      <c r="K7" t="s">
+        <v>134</v>
+      </c>
     </row>
     <row r="8" spans="1:11" ht="73.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A8" s="4" t="s">
@@ -1325,7 +1323,7 @@
         <v>71</v>
       </c>
     </row>
-    <row r="17" spans="1:10" ht="30" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:11" ht="30" x14ac:dyDescent="0.25">
       <c r="A17" s="4" t="s">
         <v>77</v>
       </c>
@@ -1350,7 +1348,7 @@
         <v>71</v>
       </c>
     </row>
-    <row r="18" spans="1:10" ht="51" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:11" ht="51" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A18" s="4" t="s">
         <v>81</v>
       </c>
@@ -1375,7 +1373,7 @@
         <v>45</v>
       </c>
     </row>
-    <row r="19" spans="1:10" ht="45" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:11" ht="45" x14ac:dyDescent="0.25">
       <c r="A19" s="4" t="s">
         <v>131</v>
       </c>
@@ -1402,7 +1400,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="20" spans="1:10" ht="48" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:11" ht="48" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A20" s="4" t="s">
         <v>84</v>
       </c>
@@ -1430,8 +1428,11 @@
       <c r="J20" t="s">
         <v>45</v>
       </c>
-    </row>
-    <row r="21" spans="1:10" ht="60" x14ac:dyDescent="0.25">
+      <c r="K20" t="s">
+        <v>134</v>
+      </c>
+    </row>
+    <row r="21" spans="1:11" ht="60" x14ac:dyDescent="0.25">
       <c r="A21" s="4" t="s">
         <v>100</v>
       </c>
@@ -1457,8 +1458,11 @@
       <c r="J21" t="s">
         <v>45</v>
       </c>
-    </row>
-    <row r="22" spans="1:10" ht="45" x14ac:dyDescent="0.25">
+      <c r="K21" t="s">
+        <v>134</v>
+      </c>
+    </row>
+    <row r="22" spans="1:11" ht="45" x14ac:dyDescent="0.25">
       <c r="A22" s="4" t="s">
         <v>102</v>
       </c>
@@ -1485,8 +1489,11 @@
       <c r="J22" t="s">
         <v>45</v>
       </c>
-    </row>
-    <row r="23" spans="1:10" ht="45" x14ac:dyDescent="0.25">
+      <c r="K22" t="s">
+        <v>134</v>
+      </c>
+    </row>
+    <row r="23" spans="1:11" ht="45" x14ac:dyDescent="0.25">
       <c r="A23" s="4" t="s">
         <v>105</v>
       </c>
@@ -1510,8 +1517,11 @@
       <c r="J23" t="s">
         <v>21</v>
       </c>
-    </row>
-    <row r="24" spans="1:10" ht="48.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="K23" t="s">
+        <v>134</v>
+      </c>
+    </row>
+    <row r="24" spans="1:11" ht="48.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A24" s="4" t="s">
         <v>127</v>
       </c>
@@ -1538,8 +1548,11 @@
       <c r="J24" t="s">
         <v>45</v>
       </c>
-    </row>
-    <row r="25" spans="1:10" ht="60" x14ac:dyDescent="0.25">
+      <c r="K24" t="s">
+        <v>134</v>
+      </c>
+    </row>
+    <row r="25" spans="1:11" ht="60" x14ac:dyDescent="0.25">
       <c r="A25" s="4" t="s">
         <v>126</v>
       </c>
@@ -1563,8 +1576,11 @@
       <c r="J25" t="s">
         <v>21</v>
       </c>
-    </row>
-    <row r="26" spans="1:10" ht="41.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="K25" t="s">
+        <v>134</v>
+      </c>
+    </row>
+    <row r="26" spans="1:11" ht="41.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A26" s="4" t="s">
         <v>125</v>
       </c>
@@ -1587,6 +1603,9 @@
       </c>
       <c r="J26" t="s">
         <v>45</v>
+      </c>
+      <c r="K26" t="s">
+        <v>134</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Se programa el dashboard para que muestre el porcentaje de avance de las tareas segun las acciones finalizadas, se puede actualizar e insertar acciones con solo presionar enter, y se programa botones para cerrar la tarea cuando esta este completada, tambien se cambian los botones del menu y se agrega uno nuevo para el archivo de tareas cerradas y cenceladas
</commit_message>
<xml_diff>
--- a/documentacion/Lista Requerimientos proyecto.xlsx
+++ b/documentacion/Lista Requerimientos proyecto.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="19029"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="19126"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\xampp\htdocs\Proyecto_ ISW-611\documentacion\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1DE16A87-AA56-42A9-8283-B18B5535FFAD}" xr6:coauthVersionLast="28" xr6:coauthVersionMax="28" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D837DCF0-97AF-47FC-8E6B-6D2C53B7A334}" xr6:coauthVersionLast="31" xr6:coauthVersionMax="31" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="20490" windowHeight="7755" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="232" uniqueCount="136">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="238" uniqueCount="141">
   <si>
     <t>Descripción</t>
   </si>
@@ -433,6 +433,21 @@
   </si>
   <si>
     <t>Listo, falta olvido contraseña</t>
+  </si>
+  <si>
+    <t>Listo, revizar la pregunta</t>
+  </si>
+  <si>
+    <t>Listo, ver si se oculta</t>
+  </si>
+  <si>
+    <t>Pendiente</t>
+  </si>
+  <si>
+    <t>Listo, ver si se oculta las tareas</t>
+  </si>
+  <si>
+    <t>Listo, falta recuperar tarea cancelada</t>
   </si>
 </sst>
 </file>
@@ -818,8 +833,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:K26"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A4" workbookViewId="0">
-      <selection activeCell="K8" sqref="K8"/>
+    <sheetView tabSelected="1" topLeftCell="A14" workbookViewId="0">
+      <selection activeCell="K14" sqref="K14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -992,6 +1007,9 @@
       <c r="J5" t="s">
         <v>15</v>
       </c>
+      <c r="K5" t="s">
+        <v>134</v>
+      </c>
     </row>
     <row r="6" spans="1:11" ht="73.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A6" s="4" t="s">
@@ -1055,7 +1073,7 @@
         <v>21</v>
       </c>
       <c r="K7" t="s">
-        <v>134</v>
+        <v>136</v>
       </c>
     </row>
     <row r="8" spans="1:11" ht="73.5" customHeight="1" x14ac:dyDescent="0.25">
@@ -1089,6 +1107,9 @@
       <c r="J8" t="s">
         <v>15</v>
       </c>
+      <c r="K8" t="s">
+        <v>137</v>
+      </c>
     </row>
     <row r="9" spans="1:11" ht="73.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A9" s="4" t="s">
@@ -1118,6 +1139,9 @@
       <c r="J9" t="s">
         <v>21</v>
       </c>
+      <c r="K9" t="s">
+        <v>138</v>
+      </c>
     </row>
     <row r="10" spans="1:11" ht="131.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A10" s="4" t="s">
@@ -1147,6 +1171,9 @@
       <c r="J10" t="s">
         <v>15</v>
       </c>
+      <c r="K10" t="s">
+        <v>139</v>
+      </c>
     </row>
     <row r="11" spans="1:11" ht="70.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A11" s="4" t="s">
@@ -1176,6 +1203,9 @@
       <c r="J11" t="s">
         <v>21</v>
       </c>
+      <c r="K11" t="s">
+        <v>134</v>
+      </c>
     </row>
     <row r="12" spans="1:11" ht="60" x14ac:dyDescent="0.25">
       <c r="A12" s="4" t="s">
@@ -1207,6 +1237,9 @@
       </c>
       <c r="J12" t="s">
         <v>45</v>
+      </c>
+      <c r="K12" t="s">
+        <v>140</v>
       </c>
     </row>
     <row r="13" spans="1:11" ht="58.5" customHeight="1" x14ac:dyDescent="0.25">

</xml_diff>

<commit_message>
Se realiza investigación de metodos de envio de correos mediante php, se logra un proyecto funcional y se trae codigo al proyecto, se experimentan pruebas e inicia la adaptación del codigo a los requerimientos del proyecto, se iniciara con recuperar contraseña
</commit_message>
<xml_diff>
--- a/documentacion/Lista Requerimientos proyecto.xlsx
+++ b/documentacion/Lista Requerimientos proyecto.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\xampp\htdocs\Proyecto_ ISW-611\documentacion\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D837DCF0-97AF-47FC-8E6B-6D2C53B7A334}" xr6:coauthVersionLast="31" xr6:coauthVersionMax="31" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E0D71859-19F4-406F-B71C-B47BDB22D419}" xr6:coauthVersionLast="31" xr6:coauthVersionMax="31" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="20490" windowHeight="7755" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="238" uniqueCount="141">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="242" uniqueCount="140">
   <si>
     <t>Descripción</t>
   </si>
@@ -445,9 +445,6 @@
   </si>
   <si>
     <t>Listo, ver si se oculta las tareas</t>
-  </si>
-  <si>
-    <t>Listo, falta recuperar tarea cancelada</t>
   </si>
 </sst>
 </file>
@@ -833,8 +830,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:K26"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A14" workbookViewId="0">
-      <selection activeCell="K14" sqref="K14"/>
+    <sheetView tabSelected="1" topLeftCell="A20" workbookViewId="0">
+      <selection activeCell="K28" sqref="K28"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1239,7 +1236,7 @@
         <v>45</v>
       </c>
       <c r="K12" t="s">
-        <v>140</v>
+        <v>134</v>
       </c>
     </row>
     <row r="13" spans="1:11" ht="58.5" customHeight="1" x14ac:dyDescent="0.25">
@@ -1273,6 +1270,9 @@
       <c r="J13" t="s">
         <v>45</v>
       </c>
+      <c r="K13" t="s">
+        <v>134</v>
+      </c>
     </row>
     <row r="14" spans="1:11" ht="69" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A14" s="4" t="s">
@@ -1330,6 +1330,9 @@
       <c r="J15" t="s">
         <v>71</v>
       </c>
+      <c r="K15" t="s">
+        <v>134</v>
+      </c>
     </row>
     <row r="16" spans="1:11" ht="42.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A16" s="4" t="s">
@@ -1380,6 +1383,9 @@
       <c r="J17" t="s">
         <v>71</v>
       </c>
+      <c r="K17" t="s">
+        <v>134</v>
+      </c>
     </row>
     <row r="18" spans="1:11" ht="51" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A18" s="4" t="s">
@@ -1404,6 +1410,9 @@
       </c>
       <c r="J18" t="s">
         <v>45</v>
+      </c>
+      <c r="K18" t="s">
+        <v>134</v>
       </c>
     </row>
     <row r="19" spans="1:11" ht="45" x14ac:dyDescent="0.25">

</xml_diff>

<commit_message>
Se mejora el codigo del correo y se ingresan validaciones para el formulario para que valide si el correo, la respuesta secreta y la contraseña sean correctas, se mejora la plantilla de correo.
</commit_message>
<xml_diff>
--- a/documentacion/Lista Requerimientos proyecto.xlsx
+++ b/documentacion/Lista Requerimientos proyecto.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\xampp\htdocs\Proyecto_ ISW-611\documentacion\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E0D71859-19F4-406F-B71C-B47BDB22D419}" xr6:coauthVersionLast="31" xr6:coauthVersionMax="31" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B303A6E2-A878-49B7-87EF-7E4FF5FBEBE1}" xr6:coauthVersionLast="31" xr6:coauthVersionMax="31" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="20490" windowHeight="7755" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="242" uniqueCount="140">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="243" uniqueCount="141">
   <si>
     <t>Descripción</t>
   </si>
@@ -445,6 +445,9 @@
   </si>
   <si>
     <t>Listo, ver si se oculta las tareas</t>
+  </si>
+  <si>
+    <t>Listo falta el cambio de pass</t>
   </si>
 </sst>
 </file>
@@ -830,8 +833,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:K26"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A20" workbookViewId="0">
-      <selection activeCell="K28" sqref="K28"/>
+    <sheetView tabSelected="1" topLeftCell="A3" workbookViewId="0">
+      <selection activeCell="K5" sqref="K5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -974,6 +977,9 @@
       <c r="J4" t="s">
         <v>21</v>
       </c>
+      <c r="K4" t="s">
+        <v>140</v>
+      </c>
     </row>
     <row r="5" spans="1:11" ht="73.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A5" s="4" t="s">

</xml_diff>